<commit_message>
Finish compare price and put the cheaptest into the WinePrice
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/wineprice/09 23 15 Grand Cru Price List.xlsx
+++ b/src/main/webapp/WEB-INF/wineprice/09 23 15 Grand Cru Price List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesHo\Downloads\"/>
     </mc:Choice>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2851" uniqueCount="519">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2855" uniqueCount="523">
   <si>
     <t>BORDEAUX</t>
   </si>
@@ -1578,6 +1578,18 @@
   </si>
   <si>
     <t>33250 Pauillac (France)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Vintage</t>
+  </si>
+  <si>
+    <t>Bottle Size</t>
+  </si>
+  <si>
+    <t>Price Euro</t>
   </si>
 </sst>
 </file>
@@ -1592,7 +1604,7 @@
   <fonts count="6">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2339,12 +2351,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="10.199999999999999"/>
   <cols>
-    <col min="1" max="1" width="26.75" style="6" customWidth="1"/>
-    <col min="2" max="2" width="13.75" style="7" customWidth="1"/>
-    <col min="3" max="3" width="8.75" style="8" customWidth="1"/>
-    <col min="4" max="4" width="8.25" style="9" customWidth="1"/>
-    <col min="5" max="6" width="10.25" style="10" customWidth="1"/>
-    <col min="7" max="16384" width="11.375" style="12"/>
+    <col min="1" max="1" customWidth="true" style="6" width="26.75" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="7" width="13.75" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="8" width="8.75" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="9" width="8.25" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" style="10" width="10.25" collapsed="true"/>
+    <col min="7" max="16384" style="12" width="11.375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35.4">
@@ -2372,15 +2384,21 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>519</v>
+      </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>521</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>504</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>505</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -30022,7 +30040,7 @@
   <pageMargins left="0.78740157480314998" right="0.78740157480314998" top="0.39370078740157499" bottom="0.39370078740157499" header="0.27559055118110198" footer="0.196850393700787"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;L&amp;"Times New Roman,Normal"&amp;8&amp;D&amp;R&amp;"Times New Roman,Normal"&amp;8Page &amp;P sur &amp;N</oddFooter>
+    <oddFooter><![CDATA[&L&"Times New Roman,Normal"&8&D&R&"Times New Roman,Normal"&8Page &P sur &N]]></oddFooter>
   </headerFooter>
 </worksheet>
 </file>

</xml_diff>